<commit_message>
Nova versão do IG
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-BRAtestado.xlsx
+++ b/docs/StructureDefinition-BRAtestado.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-07T18:11:02-03:00</t>
+    <t>2024-02-08T18:05:18-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Deploy with publisher 1.6.31
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-BRAtestado.xlsx
+++ b/docs/StructureDefinition-BRAtestado.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-22T16:03:25-03:00</t>
+    <t>2024-10-15T16:51:50-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,7 +72,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>null (http://www.saude.gov.br)</t>
   </si>
   <si>
     <t>Jurisdiction</t>

</xml_diff>